<commit_message>
Je ne sais pas ce que j'ai fait :^)
</commit_message>
<xml_diff>
--- a/Squelette_sujet_GUI/Squelette_sujet_GUI.xlsx
+++ b/Squelette_sujet_GUI/Squelette_sujet_GUI.xlsx
@@ -13,7 +13,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="548" uniqueCount="67">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="707" uniqueCount="67">
   <si>
     <t>Stimulus</t>
   </si>
@@ -234,7 +234,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="19">
+  <borders count="29">
     <border>
       <left/>
       <right/>
@@ -260,11 +260,21 @@
     <border/>
     <border/>
     <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="19">
+  <cellXfs count="29">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="true"/>
     <xf numFmtId="22" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="true"/>
@@ -284,6 +294,16 @@
     <xf numFmtId="22" fontId="0" fillId="0" borderId="16" xfId="0" applyNumberFormat="true"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="17" xfId="0" applyNumberFormat="true"/>
     <xf numFmtId="22" fontId="0" fillId="0" borderId="18" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="19" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="20" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="21" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="22" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="23" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="24" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="25" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="26" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="27" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="28" xfId="0" applyNumberFormat="true"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -308,112 +328,112 @@
   </cols>
   <sheetData>
     <row r="1">
-      <c r="A1" s="17" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="17" t="s">
+      <c r="A1" s="27" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="27" t="s">
         <v>3</v>
       </c>
-      <c r="C1" s="17" t="s">
+      <c r="C1" s="27" t="s">
         <v>6</v>
       </c>
-      <c r="D1" s="17" t="s">
+      <c r="D1" s="27" t="s">
         <v>9</v>
       </c>
-      <c r="E1" s="17" t="s">
+      <c r="E1" s="27" t="s">
         <v>12</v>
       </c>
-      <c r="F1" s="17" t="s">
+      <c r="F1" s="27" t="s">
         <v>15</v>
       </c>
-      <c r="G1" s="17" t="s">
+      <c r="G1" s="27" t="s">
         <v>16</v>
       </c>
-      <c r="H1" s="17" t="s">
+      <c r="H1" s="27" t="s">
         <v>18</v>
       </c>
-      <c r="I1" s="17" t="s">
+      <c r="I1" s="27" t="s">
         <v>64</v>
       </c>
     </row>
     <row r="2">
-      <c r="A2" s="17" t="s">
+      <c r="A2" s="27" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="17" t="s">
-        <v>11</v>
-      </c>
-      <c r="C2" s="17" t="s">
+      <c r="B2" s="27" t="s">
+        <v>4</v>
+      </c>
+      <c r="C2" s="27" t="s">
         <v>30</v>
       </c>
-      <c r="D2" s="17" t="s">
-        <v>24</v>
-      </c>
-      <c r="E2" s="17" t="s">
+      <c r="D2" s="27" t="s">
+        <v>24</v>
+      </c>
+      <c r="E2" s="27" t="s">
         <v>26</v>
       </c>
       <c r="F2">
-        <v>0.26198770012706518</v>
-      </c>
-      <c r="G2" s="17" t="s">
+        <v>0.55123929958790541</v>
+      </c>
+      <c r="G2" s="27" t="s">
+        <v>17</v>
+      </c>
+      <c r="H2" t="b">
+        <v>0</v>
+      </c>
+      <c r="I2" s="21">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" s="27" t="s">
+        <v>2</v>
+      </c>
+      <c r="B3" s="27" t="s">
+        <v>24</v>
+      </c>
+      <c r="C3" s="27" t="s">
+        <v>32</v>
+      </c>
+      <c r="D3" s="27" t="s">
+        <v>11</v>
+      </c>
+      <c r="E3" s="27" t="s">
+        <v>29</v>
+      </c>
+      <c r="F3">
+        <v>0.32048070011660457</v>
+      </c>
+      <c r="G3" s="27" t="s">
         <v>33</v>
       </c>
-      <c r="H2" t="b">
-        <v>0</v>
-      </c>
-      <c r="I2" s="17" t="s">
+      <c r="H3" t="b">
+        <v>0</v>
+      </c>
+      <c r="I3" s="27" t="s">
         <v>65</v>
       </c>
     </row>
-    <row r="3">
-      <c r="A3" s="17" t="s">
-        <v>2</v>
-      </c>
-      <c r="B3" s="17" t="s">
-        <v>24</v>
-      </c>
-      <c r="C3" s="17" t="s">
-        <v>34</v>
-      </c>
-      <c r="D3" s="17" t="s">
+    <row r="4">
+      <c r="A4" s="27" t="s">
+        <v>19</v>
+      </c>
+      <c r="B4" s="27" t="s">
         <v>4</v>
       </c>
-      <c r="E3" s="17" t="s">
-        <v>36</v>
-      </c>
-      <c r="F3">
-        <v>0.14530900027602911</v>
-      </c>
-      <c r="G3" s="17" t="s">
-        <v>33</v>
-      </c>
-      <c r="H3" t="b">
-        <v>0</v>
-      </c>
-      <c r="I3" s="17" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="4">
-      <c r="A4" s="15" t="s">
-        <v>19</v>
-      </c>
-      <c r="B4" s="15" t="s">
-        <v>5</v>
-      </c>
-      <c r="C4" s="15" t="s">
-        <v>8</v>
-      </c>
-      <c r="D4" s="15" t="s">
-        <v>5</v>
-      </c>
-      <c r="E4" s="15" t="s">
-        <v>8</v>
+      <c r="C4" s="27" t="s">
+        <v>63</v>
+      </c>
+      <c r="D4" s="27" t="s">
+        <v>11</v>
+      </c>
+      <c r="E4" s="27" t="s">
+        <v>63</v>
       </c>
       <c r="F4">
-        <v>0.41102480003610253</v>
-      </c>
-      <c r="G4" s="15" t="s">
+        <v>0.24390819994732738</v>
+      </c>
+      <c r="G4" s="27" t="s">
         <v>33</v>
       </c>
       <c r="H4" t="b">
@@ -424,83 +444,83 @@
       </c>
     </row>
     <row r="5">
-      <c r="A5" s="15" t="s">
+      <c r="A5" s="25" t="s">
         <v>20</v>
       </c>
-      <c r="B5" s="15" t="s">
-        <v>24</v>
-      </c>
-      <c r="C5" s="15" t="s">
-        <v>25</v>
-      </c>
-      <c r="D5" s="15" t="s">
+      <c r="B5" s="25" t="s">
         <v>5</v>
       </c>
-      <c r="E5" s="15" t="s">
-        <v>25</v>
+      <c r="C5" s="25" t="s">
+        <v>56</v>
+      </c>
+      <c r="D5" s="25" t="s">
+        <v>11</v>
+      </c>
+      <c r="E5" s="25" t="s">
+        <v>63</v>
       </c>
       <c r="F5">
-        <v>0.78922679973766208</v>
-      </c>
-      <c r="G5" s="15" t="s">
+        <v>0.11610620003193617</v>
+      </c>
+      <c r="G5" s="25" t="s">
         <v>33</v>
       </c>
       <c r="H5" t="b">
+        <v>0</v>
+      </c>
+      <c r="I5" s="25" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" s="21" t="s">
+        <v>21</v>
+      </c>
+      <c r="B6" s="21" t="s">
+        <v>11</v>
+      </c>
+      <c r="C6" s="21" t="s">
+        <v>36</v>
+      </c>
+      <c r="D6" s="21" t="s">
+        <v>4</v>
+      </c>
+      <c r="E6" s="21" t="s">
+        <v>36</v>
+      </c>
+      <c r="F6">
+        <v>0.12392310006543994</v>
+      </c>
+      <c r="G6" s="21" t="s">
+        <v>33</v>
+      </c>
+      <c r="H6" t="b">
         <v>1</v>
       </c>
-      <c r="I5" s="13">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="6">
-      <c r="A6" s="15" t="s">
-        <v>21</v>
-      </c>
-      <c r="B6" s="15" t="s">
-        <v>11</v>
-      </c>
-      <c r="C6" s="15" t="s">
-        <v>30</v>
-      </c>
-      <c r="D6" s="15" t="s">
-        <v>24</v>
-      </c>
-      <c r="E6" s="15" t="s">
-        <v>26</v>
-      </c>
-      <c r="F6">
-        <v>0.58203129982575774</v>
-      </c>
-      <c r="G6" s="15" t="s">
-        <v>33</v>
-      </c>
-      <c r="H6" t="b">
-        <v>0</v>
-      </c>
-      <c r="I6" s="15" t="s">
-        <v>65</v>
+      <c r="I6" s="15">
+        <v>0</v>
       </c>
     </row>
     <row r="7">
-      <c r="A7" s="15" t="s">
+      <c r="A7" s="21" t="s">
         <v>22</v>
       </c>
-      <c r="B7" s="15" t="s">
+      <c r="B7" s="21" t="s">
         <v>54</v>
       </c>
-      <c r="C7" s="15" t="s">
+      <c r="C7" s="21" t="s">
         <v>31</v>
       </c>
-      <c r="D7" s="15" t="s">
-        <v>11</v>
-      </c>
-      <c r="E7" s="15" t="s">
+      <c r="D7" s="21" t="s">
+        <v>4</v>
+      </c>
+      <c r="E7" s="21" t="s">
         <v>27</v>
       </c>
       <c r="F7">
-        <v>0.29163980018347502</v>
-      </c>
-      <c r="G7" s="15" t="s">
+        <v>0.11836670013144612</v>
+      </c>
+      <c r="G7" s="21" t="s">
         <v>17</v>
       </c>
       <c r="H7" t="b">
@@ -511,32 +531,32 @@
       </c>
     </row>
     <row r="8">
-      <c r="A8" s="15" t="s">
+      <c r="A8" s="21" t="s">
         <v>23</v>
       </c>
-      <c r="B8" s="15" t="s">
-        <v>11</v>
-      </c>
-      <c r="C8" s="15" t="s">
-        <v>62</v>
-      </c>
-      <c r="D8" s="15" t="s">
-        <v>11</v>
-      </c>
-      <c r="E8" s="15" t="s">
-        <v>62</v>
+      <c r="B8" s="21" t="s">
+        <v>5</v>
+      </c>
+      <c r="C8" s="21" t="s">
+        <v>8</v>
+      </c>
+      <c r="D8" s="21" t="s">
+        <v>24</v>
+      </c>
+      <c r="E8" s="21" t="s">
+        <v>8</v>
       </c>
       <c r="F8">
-        <v>0.2970618000254035</v>
-      </c>
-      <c r="G8" s="15" t="s">
-        <v>33</v>
+        <v>0.21273950021713972</v>
+      </c>
+      <c r="G8" s="21" t="s">
+        <v>17</v>
       </c>
       <c r="H8" t="b">
         <v>1</v>
       </c>
-      <c r="I8">
-        <v>0</v>
+      <c r="I8" s="21" t="s">
+        <v>65</v>
       </c>
     </row>
     <row r="9">

</xml_diff>

<commit_message>
J'ai fait un ratio de la police
</commit_message>
<xml_diff>
--- a/Squelette_sujet_GUI/Squelette_sujet_GUI.xlsx
+++ b/Squelette_sujet_GUI/Squelette_sujet_GUI.xlsx
@@ -13,7 +13,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1042" uniqueCount="55">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1093" uniqueCount="55">
   <si>
     <t>Stimulus</t>
   </si>
@@ -198,7 +198,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="93">
+  <borders count="97">
     <border>
       <left/>
       <right/>
@@ -298,11 +298,15 @@
     <border/>
     <border/>
     <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="93">
+  <cellXfs count="97">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="true"/>
     <xf numFmtId="22" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="true"/>
@@ -396,6 +400,10 @@
     <xf numFmtId="22" fontId="0" fillId="0" borderId="90" xfId="0" applyNumberFormat="true"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="91" xfId="0" applyNumberFormat="true"/>
     <xf numFmtId="22" fontId="0" fillId="0" borderId="92" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="93" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="94" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="95" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="96" xfId="0" applyNumberFormat="true"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -408,130 +416,130 @@
   <dimension ref="A1:I14"/>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="8.85546875" customWidth="true"/>
+    <col min="1" max="1" width="21.42578125" customWidth="true"/>
     <col min="2" max="2" width="17" customWidth="true"/>
     <col min="3" max="3" width="10" customWidth="true"/>
     <col min="4" max="4" width="18.85546875" customWidth="true"/>
     <col min="5" max="5" width="11.85546875" customWidth="true"/>
-    <col min="6" max="6" width="3.28515625" customWidth="true"/>
+    <col min="6" max="6" width="9.7109375" customWidth="true"/>
     <col min="7" max="7" width="6.42578125" customWidth="true"/>
     <col min="8" max="8" width="11.7109375" customWidth="true"/>
-    <col min="9" max="9" width="6.5703125" customWidth="true"/>
+    <col min="9" max="9" width="7.85546875" customWidth="true"/>
   </cols>
   <sheetData>
     <row r="1">
-      <c r="A1" s="91" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="91" t="s">
+      <c r="A1" s="95" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="95" t="s">
         <v>14</v>
       </c>
-      <c r="C1" s="91" t="s">
+      <c r="C1" s="95" t="s">
         <v>20</v>
       </c>
-      <c r="D1" s="91" t="s">
+      <c r="D1" s="95" t="s">
         <v>34</v>
       </c>
-      <c r="E1" s="91" t="s">
+      <c r="E1" s="95" t="s">
         <v>36</v>
       </c>
-      <c r="F1" s="91" t="s">
+      <c r="F1" s="95" t="s">
         <v>41</v>
       </c>
-      <c r="G1" s="91" t="s">
+      <c r="G1" s="95" t="s">
         <v>42</v>
       </c>
-      <c r="H1" s="91" t="s">
+      <c r="H1" s="95" t="s">
         <v>45</v>
       </c>
-      <c r="I1" s="91" t="s">
+      <c r="I1" s="95" t="s">
         <v>46</v>
       </c>
     </row>
     <row r="2">
-      <c r="A2" s="91" t="s">
+      <c r="A2" s="95" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="91" t="s">
-        <v>15</v>
-      </c>
-      <c r="C2" s="91" t="s">
-        <v>21</v>
-      </c>
-      <c r="D2" s="91" t="s">
+      <c r="B2" s="95" t="s">
         <v>19</v>
       </c>
-      <c r="E2" s="91" t="s">
-        <v>37</v>
+      <c r="C2" s="95" t="s">
+        <v>32</v>
+      </c>
+      <c r="D2" s="95" t="s">
+        <v>16</v>
+      </c>
+      <c r="E2" s="95" t="s">
+        <v>32</v>
       </c>
       <c r="F2">
-        <v>0.22528040001634508</v>
-      </c>
-      <c r="G2" s="91" t="s">
+        <v>0.25228689995128661</v>
+      </c>
+      <c r="G2" s="95" t="s">
+        <v>43</v>
+      </c>
+      <c r="H2" t="b">
+        <v>1</v>
+      </c>
+      <c r="I2" s="95" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" s="95" t="s">
+        <v>2</v>
+      </c>
+      <c r="B3" s="95" t="s">
+        <v>17</v>
+      </c>
+      <c r="C3" s="95" t="s">
+        <v>28</v>
+      </c>
+      <c r="D3" s="95" t="s">
+        <v>17</v>
+      </c>
+      <c r="E3" s="95" t="s">
+        <v>28</v>
+      </c>
+      <c r="F3">
+        <v>0.31216610001865774</v>
+      </c>
+      <c r="G3" s="95" t="s">
         <v>44</v>
-      </c>
-      <c r="H2" t="b">
-        <v>0</v>
-      </c>
-      <c r="I2" s="91" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="3">
-      <c r="A3" s="89" t="s">
-        <v>2</v>
-      </c>
-      <c r="B3" s="89" t="s">
-        <v>35</v>
-      </c>
-      <c r="C3" s="89" t="s">
-        <v>24</v>
-      </c>
-      <c r="D3" s="89" t="s">
-        <v>18</v>
-      </c>
-      <c r="E3" s="89" t="s">
-        <v>24</v>
-      </c>
-      <c r="F3">
-        <v>0.33460189995821565</v>
-      </c>
-      <c r="G3" s="89" t="s">
-        <v>43</v>
       </c>
       <c r="H3" t="b">
         <v>1</v>
       </c>
-      <c r="I3" s="89" t="s">
-        <v>48</v>
+      <c r="I3" s="89">
+        <v>0</v>
       </c>
     </row>
     <row r="4">
-      <c r="A4" s="79" t="s">
+      <c r="A4" s="95" t="s">
         <v>3</v>
       </c>
-      <c r="B4" s="79" t="s">
+      <c r="B4" s="95" t="s">
         <v>17</v>
       </c>
-      <c r="C4" s="79" t="s">
-        <v>23</v>
-      </c>
-      <c r="D4" s="79" t="s">
-        <v>15</v>
-      </c>
-      <c r="E4" s="79" t="s">
-        <v>23</v>
+      <c r="C4" s="95" t="s">
+        <v>52</v>
+      </c>
+      <c r="D4" s="95" t="s">
+        <v>16</v>
+      </c>
+      <c r="E4" s="95" t="s">
+        <v>49</v>
       </c>
       <c r="F4">
-        <v>4.8969378999900073</v>
-      </c>
-      <c r="G4" s="79" t="s">
-        <v>43</v>
+        <v>0.4446981999790296</v>
+      </c>
+      <c r="G4" s="95" t="s">
+        <v>44</v>
       </c>
       <c r="H4" t="b">
-        <v>1</v>
-      </c>
-      <c r="I4" s="79" t="s">
+        <v>0</v>
+      </c>
+      <c r="I4" s="95" t="s">
         <v>48</v>
       </c>
     </row>

</xml_diff>

<commit_message>
fuck les opérateurs logiques
</commit_message>
<xml_diff>
--- a/Squelette_sujet_GUI/Squelette_sujet_GUI.xlsx
+++ b/Squelette_sujet_GUI/Squelette_sujet_GUI.xlsx
@@ -13,7 +13,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1093" uniqueCount="55">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1123" uniqueCount="55">
   <si>
     <t>Stimulus</t>
   </si>
@@ -198,7 +198,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="97">
+  <borders count="101">
     <border>
       <left/>
       <right/>
@@ -302,11 +302,15 @@
     <border/>
     <border/>
     <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="97">
+  <cellXfs count="101">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="true"/>
     <xf numFmtId="22" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="true"/>
@@ -404,6 +408,10 @@
     <xf numFmtId="22" fontId="0" fillId="0" borderId="94" xfId="0" applyNumberFormat="true"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="95" xfId="0" applyNumberFormat="true"/>
     <xf numFmtId="22" fontId="0" fillId="0" borderId="96" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="97" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="98" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="99" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="100" xfId="0" applyNumberFormat="true"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -416,73 +424,73 @@
   <dimension ref="A1:I14"/>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="21.42578125" customWidth="true"/>
+    <col min="1" max="1" width="8.85546875" customWidth="true"/>
     <col min="2" max="2" width="17" customWidth="true"/>
     <col min="3" max="3" width="10" customWidth="true"/>
     <col min="4" max="4" width="18.85546875" customWidth="true"/>
     <col min="5" max="5" width="11.85546875" customWidth="true"/>
-    <col min="6" max="6" width="9.7109375" customWidth="true"/>
+    <col min="6" max="6" width="3.28515625" customWidth="true"/>
     <col min="7" max="7" width="6.42578125" customWidth="true"/>
     <col min="8" max="8" width="11.7109375" customWidth="true"/>
-    <col min="9" max="9" width="7.85546875" customWidth="true"/>
+    <col min="9" max="9" width="6.5703125" customWidth="true"/>
   </cols>
   <sheetData>
     <row r="1">
-      <c r="A1" s="95" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="95" t="s">
+      <c r="A1" s="99" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="99" t="s">
         <v>14</v>
       </c>
-      <c r="C1" s="95" t="s">
+      <c r="C1" s="99" t="s">
         <v>20</v>
       </c>
-      <c r="D1" s="95" t="s">
+      <c r="D1" s="99" t="s">
         <v>34</v>
       </c>
-      <c r="E1" s="95" t="s">
+      <c r="E1" s="99" t="s">
         <v>36</v>
       </c>
-      <c r="F1" s="95" t="s">
+      <c r="F1" s="99" t="s">
         <v>41</v>
       </c>
-      <c r="G1" s="95" t="s">
+      <c r="G1" s="99" t="s">
         <v>42</v>
       </c>
-      <c r="H1" s="95" t="s">
+      <c r="H1" s="99" t="s">
         <v>45</v>
       </c>
-      <c r="I1" s="95" t="s">
+      <c r="I1" s="99" t="s">
         <v>46</v>
       </c>
     </row>
     <row r="2">
-      <c r="A2" s="95" t="s">
+      <c r="A2" s="99" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="95" t="s">
-        <v>19</v>
-      </c>
-      <c r="C2" s="95" t="s">
-        <v>32</v>
-      </c>
-      <c r="D2" s="95" t="s">
-        <v>16</v>
-      </c>
-      <c r="E2" s="95" t="s">
-        <v>32</v>
+      <c r="B2" s="99" t="s">
+        <v>16</v>
+      </c>
+      <c r="C2" s="99" t="s">
+        <v>27</v>
+      </c>
+      <c r="D2" s="99" t="s">
+        <v>18</v>
+      </c>
+      <c r="E2" s="99" t="s">
+        <v>24</v>
       </c>
       <c r="F2">
-        <v>0.25228689995128661</v>
-      </c>
-      <c r="G2" s="95" t="s">
+        <v>0.2253749999217689</v>
+      </c>
+      <c r="G2" s="99" t="s">
         <v>43</v>
       </c>
       <c r="H2" t="b">
-        <v>1</v>
-      </c>
-      <c r="I2" s="95" t="s">
-        <v>48</v>
+        <v>0</v>
+      </c>
+      <c r="I2" s="95">
+        <v>0</v>
       </c>
     </row>
     <row r="3">

</xml_diff>

<commit_message>
petit bug de réglé
</commit_message>
<xml_diff>
--- a/Squelette_sujet_GUI/Squelette_sujet_GUI.xlsx
+++ b/Squelette_sujet_GUI/Squelette_sujet_GUI.xlsx
@@ -13,7 +13,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1123" uniqueCount="55">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1159" uniqueCount="55">
   <si>
     <t>Stimulus</t>
   </si>
@@ -198,7 +198,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="101">
+  <borders count="105">
     <border>
       <left/>
       <right/>
@@ -306,11 +306,15 @@
     <border/>
     <border/>
     <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="101">
+  <cellXfs count="105">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="true"/>
     <xf numFmtId="22" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="true"/>
@@ -412,6 +416,10 @@
     <xf numFmtId="22" fontId="0" fillId="0" borderId="98" xfId="0" applyNumberFormat="true"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="99" xfId="0" applyNumberFormat="true"/>
     <xf numFmtId="22" fontId="0" fillId="0" borderId="100" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="101" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="102" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="103" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="104" xfId="0" applyNumberFormat="true"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -436,54 +444,54 @@
   </cols>
   <sheetData>
     <row r="1">
-      <c r="A1" s="99" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="99" t="s">
+      <c r="A1" s="103" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="103" t="s">
         <v>14</v>
       </c>
-      <c r="C1" s="99" t="s">
+      <c r="C1" s="103" t="s">
         <v>20</v>
       </c>
-      <c r="D1" s="99" t="s">
+      <c r="D1" s="103" t="s">
         <v>34</v>
       </c>
-      <c r="E1" s="99" t="s">
+      <c r="E1" s="103" t="s">
         <v>36</v>
       </c>
-      <c r="F1" s="99" t="s">
+      <c r="F1" s="103" t="s">
         <v>41</v>
       </c>
-      <c r="G1" s="99" t="s">
+      <c r="G1" s="103" t="s">
         <v>42</v>
       </c>
-      <c r="H1" s="99" t="s">
+      <c r="H1" s="103" t="s">
         <v>45</v>
       </c>
-      <c r="I1" s="99" t="s">
+      <c r="I1" s="103" t="s">
         <v>46</v>
       </c>
     </row>
     <row r="2">
-      <c r="A2" s="99" t="s">
+      <c r="A2" s="103" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="99" t="s">
-        <v>16</v>
-      </c>
-      <c r="C2" s="99" t="s">
-        <v>27</v>
-      </c>
-      <c r="D2" s="99" t="s">
-        <v>18</v>
-      </c>
-      <c r="E2" s="99" t="s">
-        <v>24</v>
+      <c r="B2" s="103" t="s">
+        <v>19</v>
+      </c>
+      <c r="C2" s="103" t="s">
+        <v>47</v>
+      </c>
+      <c r="D2" s="103" t="s">
+        <v>35</v>
+      </c>
+      <c r="E2" s="103" t="s">
+        <v>54</v>
       </c>
       <c r="F2">
-        <v>0.2253749999217689</v>
-      </c>
-      <c r="G2" s="99" t="s">
+        <v>0.56456759991124272</v>
+      </c>
+      <c r="G2" s="103" t="s">
         <v>43</v>
       </c>
       <c r="H2" t="b">
@@ -494,25 +502,25 @@
       </c>
     </row>
     <row r="3">
-      <c r="A3" s="95" t="s">
+      <c r="A3" s="101" t="s">
         <v>2</v>
       </c>
-      <c r="B3" s="95" t="s">
-        <v>17</v>
-      </c>
-      <c r="C3" s="95" t="s">
-        <v>28</v>
-      </c>
-      <c r="D3" s="95" t="s">
-        <v>17</v>
-      </c>
-      <c r="E3" s="95" t="s">
-        <v>28</v>
+      <c r="B3" s="101" t="s">
+        <v>19</v>
+      </c>
+      <c r="C3" s="101" t="s">
+        <v>25</v>
+      </c>
+      <c r="D3" s="101" t="s">
+        <v>19</v>
+      </c>
+      <c r="E3" s="101" t="s">
+        <v>25</v>
       </c>
       <c r="F3">
-        <v>0.31216610001865774</v>
-      </c>
-      <c r="G3" s="95" t="s">
+        <v>0.58663499995600432</v>
+      </c>
+      <c r="G3" s="101" t="s">
         <v>44</v>
       </c>
       <c r="H3" t="b">

</xml_diff>

<commit_message>
AHHHHH I hate it all
</commit_message>
<xml_diff>
--- a/Squelette_sujet_GUI/Squelette_sujet_GUI.xlsx
+++ b/Squelette_sujet_GUI/Squelette_sujet_GUI.xlsx
@@ -13,7 +13,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1159" uniqueCount="55">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1193" uniqueCount="55">
   <si>
     <t>Stimulus</t>
   </si>
@@ -198,7 +198,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="105">
+  <borders count="107">
     <border>
       <left/>
       <right/>
@@ -310,11 +310,13 @@
     <border/>
     <border/>
     <border/>
+    <border/>
+    <border/>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="105">
+  <cellXfs count="107">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="true"/>
     <xf numFmtId="22" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="true"/>
@@ -420,6 +422,8 @@
     <xf numFmtId="22" fontId="0" fillId="0" borderId="102" xfId="0" applyNumberFormat="true"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="103" xfId="0" applyNumberFormat="true"/>
     <xf numFmtId="22" fontId="0" fillId="0" borderId="104" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="105" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="106" xfId="0" applyNumberFormat="true"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -432,66 +436,66 @@
   <dimension ref="A1:I14"/>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="8.85546875" customWidth="true"/>
+    <col min="1" max="1" width="21.42578125" customWidth="true"/>
     <col min="2" max="2" width="17" customWidth="true"/>
     <col min="3" max="3" width="10" customWidth="true"/>
     <col min="4" max="4" width="18.85546875" customWidth="true"/>
     <col min="5" max="5" width="11.85546875" customWidth="true"/>
-    <col min="6" max="6" width="3.28515625" customWidth="true"/>
+    <col min="6" max="6" width="9.7109375" customWidth="true"/>
     <col min="7" max="7" width="6.42578125" customWidth="true"/>
     <col min="8" max="8" width="11.7109375" customWidth="true"/>
     <col min="9" max="9" width="6.5703125" customWidth="true"/>
   </cols>
   <sheetData>
     <row r="1">
-      <c r="A1" s="103" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="103" t="s">
+      <c r="A1" s="105" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="105" t="s">
         <v>14</v>
       </c>
-      <c r="C1" s="103" t="s">
+      <c r="C1" s="105" t="s">
         <v>20</v>
       </c>
-      <c r="D1" s="103" t="s">
+      <c r="D1" s="105" t="s">
         <v>34</v>
       </c>
-      <c r="E1" s="103" t="s">
+      <c r="E1" s="105" t="s">
         <v>36</v>
       </c>
-      <c r="F1" s="103" t="s">
+      <c r="F1" s="105" t="s">
         <v>41</v>
       </c>
-      <c r="G1" s="103" t="s">
+      <c r="G1" s="105" t="s">
         <v>42</v>
       </c>
-      <c r="H1" s="103" t="s">
+      <c r="H1" s="105" t="s">
         <v>45</v>
       </c>
-      <c r="I1" s="103" t="s">
+      <c r="I1" s="105" t="s">
         <v>46</v>
       </c>
     </row>
     <row r="2">
-      <c r="A2" s="103" t="s">
+      <c r="A2" s="105" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="103" t="s">
+      <c r="B2" s="105" t="s">
         <v>19</v>
       </c>
-      <c r="C2" s="103" t="s">
-        <v>47</v>
-      </c>
-      <c r="D2" s="103" t="s">
+      <c r="C2" s="105" t="s">
+        <v>27</v>
+      </c>
+      <c r="D2" s="105" t="s">
         <v>35</v>
       </c>
-      <c r="E2" s="103" t="s">
-        <v>54</v>
+      <c r="E2" s="105" t="s">
+        <v>24</v>
       </c>
       <c r="F2">
-        <v>0.56456759991124272</v>
-      </c>
-      <c r="G2" s="103" t="s">
+        <v>0.39905829995404929</v>
+      </c>
+      <c r="G2" s="105" t="s">
         <v>43</v>
       </c>
       <c r="H2" t="b">
@@ -502,89 +506,89 @@
       </c>
     </row>
     <row r="3">
-      <c r="A3" s="101" t="s">
+      <c r="A3" s="105" t="s">
         <v>2</v>
       </c>
-      <c r="B3" s="101" t="s">
+      <c r="B3" s="105" t="s">
+        <v>16</v>
+      </c>
+      <c r="C3" s="105" t="s">
+        <v>30</v>
+      </c>
+      <c r="D3" s="105" t="s">
+        <v>15</v>
+      </c>
+      <c r="E3" s="105" t="s">
+        <v>53</v>
+      </c>
+      <c r="F3">
+        <v>0.42982720001600683</v>
+      </c>
+      <c r="G3" s="105" t="s">
+        <v>43</v>
+      </c>
+      <c r="H3" t="b">
+        <v>0</v>
+      </c>
+      <c r="I3" s="89">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" s="105" t="s">
+        <v>3</v>
+      </c>
+      <c r="B4" s="105" t="s">
+        <v>15</v>
+      </c>
+      <c r="C4" s="105" t="s">
+        <v>40</v>
+      </c>
+      <c r="D4" s="105" t="s">
+        <v>16</v>
+      </c>
+      <c r="E4" s="105" t="s">
+        <v>33</v>
+      </c>
+      <c r="F4">
+        <v>0.364127799984999</v>
+      </c>
+      <c r="G4" s="105" t="s">
+        <v>43</v>
+      </c>
+      <c r="H4" t="b">
+        <v>0</v>
+      </c>
+      <c r="I4" s="95">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" s="105" t="s">
+        <v>4</v>
+      </c>
+      <c r="B5" s="105" t="s">
         <v>19</v>
       </c>
-      <c r="C3" s="101" t="s">
+      <c r="C5" s="105" t="s">
         <v>25</v>
       </c>
-      <c r="D3" s="101" t="s">
+      <c r="D5" s="105" t="s">
         <v>19</v>
       </c>
-      <c r="E3" s="101" t="s">
+      <c r="E5" s="105" t="s">
         <v>25</v>
       </c>
-      <c r="F3">
-        <v>0.58663499995600432</v>
-      </c>
-      <c r="G3" s="101" t="s">
-        <v>44</v>
-      </c>
-      <c r="H3" t="b">
+      <c r="F5">
+        <v>0.41065490001346916</v>
+      </c>
+      <c r="G5" s="105" t="s">
+        <v>43</v>
+      </c>
+      <c r="H5" t="b">
         <v>1</v>
       </c>
-      <c r="I3" s="89">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="4">
-      <c r="A4" s="95" t="s">
-        <v>3</v>
-      </c>
-      <c r="B4" s="95" t="s">
-        <v>17</v>
-      </c>
-      <c r="C4" s="95" t="s">
-        <v>52</v>
-      </c>
-      <c r="D4" s="95" t="s">
-        <v>16</v>
-      </c>
-      <c r="E4" s="95" t="s">
-        <v>49</v>
-      </c>
-      <c r="F4">
-        <v>0.4446981999790296</v>
-      </c>
-      <c r="G4" s="95" t="s">
-        <v>44</v>
-      </c>
-      <c r="H4" t="b">
-        <v>0</v>
-      </c>
-      <c r="I4" s="95" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="5">
-      <c r="A5" s="71" t="s">
-        <v>4</v>
-      </c>
-      <c r="B5" s="71" t="s">
-        <v>19</v>
-      </c>
-      <c r="C5" s="71" t="s">
-        <v>37</v>
-      </c>
-      <c r="D5" s="71" t="s">
-        <v>17</v>
-      </c>
-      <c r="E5" s="71" t="s">
-        <v>21</v>
-      </c>
-      <c r="F5">
-        <v>0.77576820005197078</v>
-      </c>
-      <c r="G5" s="71" t="s">
-        <v>44</v>
-      </c>
-      <c r="H5" t="b">
-        <v>0</v>
-      </c>
-      <c r="I5" s="71" t="s">
+      <c r="I5" s="105" t="s">
         <v>48</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Je pense que c'est pas mal fini
</commit_message>
<xml_diff>
--- a/Squelette_sujet_GUI/Squelette_sujet_GUI.xlsx
+++ b/Squelette_sujet_GUI/Squelette_sujet_GUI.xlsx
@@ -13,7 +13,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1193" uniqueCount="55">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1280" uniqueCount="55">
   <si>
     <t>Stimulus</t>
   </si>
@@ -198,7 +198,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="107">
+  <borders count="115">
     <border>
       <left/>
       <right/>
@@ -312,11 +312,19 @@
     <border/>
     <border/>
     <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="107">
+  <cellXfs count="115">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="true"/>
     <xf numFmtId="22" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="true"/>
@@ -424,6 +432,14 @@
     <xf numFmtId="22" fontId="0" fillId="0" borderId="104" xfId="0" applyNumberFormat="true"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="105" xfId="0" applyNumberFormat="true"/>
     <xf numFmtId="22" fontId="0" fillId="0" borderId="106" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="107" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="108" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="109" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="110" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="111" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="112" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="113" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="114" xfId="0" applyNumberFormat="true"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -436,126 +452,126 @@
   <dimension ref="A1:I14"/>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="21.42578125" customWidth="true"/>
+    <col min="1" max="1" width="8.85546875" customWidth="true"/>
     <col min="2" max="2" width="17" customWidth="true"/>
     <col min="3" max="3" width="10" customWidth="true"/>
     <col min="4" max="4" width="18.85546875" customWidth="true"/>
     <col min="5" max="5" width="11.85546875" customWidth="true"/>
-    <col min="6" max="6" width="9.7109375" customWidth="true"/>
+    <col min="6" max="6" width="3.28515625" customWidth="true"/>
     <col min="7" max="7" width="6.42578125" customWidth="true"/>
     <col min="8" max="8" width="11.7109375" customWidth="true"/>
     <col min="9" max="9" width="6.5703125" customWidth="true"/>
   </cols>
   <sheetData>
     <row r="1">
-      <c r="A1" s="105" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="105" t="s">
+      <c r="A1" s="113" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="113" t="s">
         <v>14</v>
       </c>
-      <c r="C1" s="105" t="s">
+      <c r="C1" s="113" t="s">
         <v>20</v>
       </c>
-      <c r="D1" s="105" t="s">
+      <c r="D1" s="113" t="s">
         <v>34</v>
       </c>
-      <c r="E1" s="105" t="s">
+      <c r="E1" s="113" t="s">
         <v>36</v>
       </c>
-      <c r="F1" s="105" t="s">
+      <c r="F1" s="113" t="s">
         <v>41</v>
       </c>
-      <c r="G1" s="105" t="s">
+      <c r="G1" s="113" t="s">
         <v>42</v>
       </c>
-      <c r="H1" s="105" t="s">
+      <c r="H1" s="113" t="s">
         <v>45</v>
       </c>
-      <c r="I1" s="105" t="s">
+      <c r="I1" s="113" t="s">
         <v>46</v>
       </c>
     </row>
     <row r="2">
-      <c r="A2" s="105" t="s">
+      <c r="A2" s="113" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="105" t="s">
+      <c r="B2" s="113" t="s">
         <v>19</v>
       </c>
-      <c r="C2" s="105" t="s">
-        <v>27</v>
-      </c>
-      <c r="D2" s="105" t="s">
-        <v>35</v>
-      </c>
-      <c r="E2" s="105" t="s">
-        <v>24</v>
+      <c r="C2" s="113" t="s">
+        <v>25</v>
+      </c>
+      <c r="D2" s="113" t="s">
+        <v>15</v>
+      </c>
+      <c r="E2" s="113" t="s">
+        <v>26</v>
       </c>
       <c r="F2">
-        <v>0.39905829995404929</v>
-      </c>
-      <c r="G2" s="105" t="s">
+        <v>0.56264150002971292</v>
+      </c>
+      <c r="G2" s="113" t="s">
+        <v>44</v>
+      </c>
+      <c r="H2" t="b">
+        <v>0</v>
+      </c>
+      <c r="I2" s="113" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" s="107" t="s">
+        <v>2</v>
+      </c>
+      <c r="B3" s="107" t="s">
+        <v>17</v>
+      </c>
+      <c r="C3" s="107" t="s">
+        <v>40</v>
+      </c>
+      <c r="D3" s="107" t="s">
+        <v>19</v>
+      </c>
+      <c r="E3" s="107" t="s">
+        <v>33</v>
+      </c>
+      <c r="F3">
+        <v>0.34822820010595024</v>
+      </c>
+      <c r="G3" s="107" t="s">
         <v>43</v>
       </c>
-      <c r="H2" t="b">
-        <v>0</v>
-      </c>
-      <c r="I2" s="95">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="3">
-      <c r="A3" s="105" t="s">
-        <v>2</v>
-      </c>
-      <c r="B3" s="105" t="s">
-        <v>16</v>
-      </c>
-      <c r="C3" s="105" t="s">
-        <v>30</v>
-      </c>
-      <c r="D3" s="105" t="s">
+      <c r="H3" t="b">
+        <v>0</v>
+      </c>
+      <c r="I3" s="89">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" s="107" t="s">
+        <v>3</v>
+      </c>
+      <c r="B4" s="107" t="s">
+        <v>19</v>
+      </c>
+      <c r="C4" s="107" t="s">
+        <v>32</v>
+      </c>
+      <c r="D4" s="107" t="s">
         <v>15</v>
       </c>
-      <c r="E3" s="105" t="s">
-        <v>53</v>
-      </c>
-      <c r="F3">
-        <v>0.42982720001600683</v>
-      </c>
-      <c r="G3" s="105" t="s">
+      <c r="E4" s="107" t="s">
+        <v>23</v>
+      </c>
+      <c r="F4">
+        <v>0.22370430000592023</v>
+      </c>
+      <c r="G4" s="107" t="s">
         <v>43</v>
       </c>
-      <c r="H3" t="b">
-        <v>0</v>
-      </c>
-      <c r="I3" s="89">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="4">
-      <c r="A4" s="105" t="s">
-        <v>3</v>
-      </c>
-      <c r="B4" s="105" t="s">
-        <v>15</v>
-      </c>
-      <c r="C4" s="105" t="s">
-        <v>40</v>
-      </c>
-      <c r="D4" s="105" t="s">
-        <v>16</v>
-      </c>
-      <c r="E4" s="105" t="s">
-        <v>33</v>
-      </c>
-      <c r="F4">
-        <v>0.364127799984999</v>
-      </c>
-      <c r="G4" s="105" t="s">
-        <v>43</v>
-      </c>
       <c r="H4" t="b">
         <v>0</v>
       </c>
@@ -564,61 +580,61 @@
       </c>
     </row>
     <row r="5">
-      <c r="A5" s="105" t="s">
+      <c r="A5" s="107" t="s">
         <v>4</v>
       </c>
-      <c r="B5" s="105" t="s">
+      <c r="B5" s="107" t="s">
         <v>19</v>
       </c>
-      <c r="C5" s="105" t="s">
-        <v>25</v>
-      </c>
-      <c r="D5" s="105" t="s">
+      <c r="C5" s="107" t="s">
+        <v>49</v>
+      </c>
+      <c r="D5" s="107" t="s">
         <v>19</v>
       </c>
-      <c r="E5" s="105" t="s">
-        <v>25</v>
+      <c r="E5" s="107" t="s">
+        <v>49</v>
       </c>
       <c r="F5">
-        <v>0.41065490001346916</v>
-      </c>
-      <c r="G5" s="105" t="s">
+        <v>0.50990309996996075</v>
+      </c>
+      <c r="G5" s="107" t="s">
         <v>43</v>
       </c>
       <c r="H5" t="b">
         <v>1</v>
       </c>
-      <c r="I5" s="105" t="s">
+      <c r="I5" s="107" t="s">
         <v>48</v>
       </c>
     </row>
     <row r="6">
-      <c r="A6" s="71" t="s">
+      <c r="A6" s="107" t="s">
         <v>5</v>
       </c>
-      <c r="B6" s="71" t="s">
-        <v>15</v>
-      </c>
-      <c r="C6" s="71" t="s">
-        <v>23</v>
-      </c>
-      <c r="D6" s="71" t="s">
-        <v>16</v>
-      </c>
-      <c r="E6" s="71" t="s">
-        <v>32</v>
+      <c r="B6" s="107" t="s">
+        <v>17</v>
+      </c>
+      <c r="C6" s="107" t="s">
+        <v>28</v>
+      </c>
+      <c r="D6" s="107" t="s">
+        <v>19</v>
+      </c>
+      <c r="E6" s="107" t="s">
+        <v>39</v>
       </c>
       <c r="F6">
-        <v>1.6724731998983771</v>
-      </c>
-      <c r="G6" s="71" t="s">
-        <v>44</v>
+        <v>0.29754129995126277</v>
+      </c>
+      <c r="G6" s="107" t="s">
+        <v>43</v>
       </c>
       <c r="H6" t="b">
         <v>0</v>
       </c>
-      <c r="I6" s="71" t="s">
-        <v>48</v>
+      <c r="I6" s="71">
+        <v>0</v>
       </c>
     </row>
     <row r="7">

</xml_diff>

<commit_message>
J'ai reglé un bug sur les imputs
</commit_message>
<xml_diff>
--- a/Squelette_sujet_GUI/Squelette_sujet_GUI.xlsx
+++ b/Squelette_sujet_GUI/Squelette_sujet_GUI.xlsx
@@ -13,7 +13,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1280" uniqueCount="55">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1313" uniqueCount="59">
   <si>
     <t>Stimulus</t>
   </si>
@@ -178,6 +178,18 @@
   </si>
   <si>
     <t>oignon</t>
+  </si>
+  <si>
+    <t>Squelette_sujet_gui_1</t>
+  </si>
+  <si>
+    <t>Squelette_sujet_gui_2</t>
+  </si>
+  <si>
+    <t>Squelette_sujet_gui_3</t>
+  </si>
+  <si>
+    <t>Squelette_sujet_gui_4</t>
   </si>
 </sst>
 </file>
@@ -198,7 +210,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="115">
+  <borders count="117">
     <border>
       <left/>
       <right/>
@@ -320,11 +332,13 @@
     <border/>
     <border/>
     <border/>
+    <border/>
+    <border/>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="115">
+  <cellXfs count="117">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="true"/>
     <xf numFmtId="22" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="true"/>
@@ -440,6 +454,8 @@
     <xf numFmtId="22" fontId="0" fillId="0" borderId="112" xfId="0" applyNumberFormat="true"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="113" xfId="0" applyNumberFormat="true"/>
     <xf numFmtId="22" fontId="0" fillId="0" borderId="114" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="115" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="116" xfId="0" applyNumberFormat="true"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -452,160 +468,160 @@
   <dimension ref="A1:I14"/>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="8.85546875" customWidth="true"/>
+    <col min="1" max="1" width="21" customWidth="true"/>
     <col min="2" max="2" width="17" customWidth="true"/>
     <col min="3" max="3" width="10" customWidth="true"/>
     <col min="4" max="4" width="18.85546875" customWidth="true"/>
     <col min="5" max="5" width="11.85546875" customWidth="true"/>
-    <col min="6" max="6" width="3.28515625" customWidth="true"/>
+    <col min="6" max="6" width="9.7109375" customWidth="true"/>
     <col min="7" max="7" width="6.42578125" customWidth="true"/>
     <col min="8" max="8" width="11.7109375" customWidth="true"/>
     <col min="9" max="9" width="6.5703125" customWidth="true"/>
   </cols>
   <sheetData>
     <row r="1">
-      <c r="A1" s="113" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="113" t="s">
+      <c r="A1" s="115" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="115" t="s">
         <v>14</v>
       </c>
-      <c r="C1" s="113" t="s">
+      <c r="C1" s="115" t="s">
         <v>20</v>
       </c>
-      <c r="D1" s="113" t="s">
+      <c r="D1" s="115" t="s">
         <v>34</v>
       </c>
-      <c r="E1" s="113" t="s">
+      <c r="E1" s="115" t="s">
         <v>36</v>
       </c>
-      <c r="F1" s="113" t="s">
+      <c r="F1" s="115" t="s">
         <v>41</v>
       </c>
-      <c r="G1" s="113" t="s">
+      <c r="G1" s="115" t="s">
         <v>42</v>
       </c>
-      <c r="H1" s="113" t="s">
+      <c r="H1" s="115" t="s">
         <v>45</v>
       </c>
-      <c r="I1" s="113" t="s">
+      <c r="I1" s="115" t="s">
         <v>46</v>
       </c>
     </row>
     <row r="2">
-      <c r="A2" s="113" t="s">
-        <v>1</v>
-      </c>
-      <c r="B2" s="113" t="s">
+      <c r="A2" s="115" t="s">
+        <v>55</v>
+      </c>
+      <c r="B2" s="115" t="s">
+        <v>15</v>
+      </c>
+      <c r="C2" s="115" t="s">
+        <v>21</v>
+      </c>
+      <c r="D2" s="115" t="s">
+        <v>16</v>
+      </c>
+      <c r="E2" s="115" t="s">
+        <v>37</v>
+      </c>
+      <c r="F2">
+        <v>0.37934820004738867</v>
+      </c>
+      <c r="G2" s="115" t="s">
+        <v>43</v>
+      </c>
+      <c r="H2" t="b">
+        <v>0</v>
+      </c>
+      <c r="I2" s="113">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" s="115" t="s">
+        <v>56</v>
+      </c>
+      <c r="B3" s="115" t="s">
+        <v>16</v>
+      </c>
+      <c r="C3" s="115" t="s">
+        <v>22</v>
+      </c>
+      <c r="D3" s="115" t="s">
+        <v>17</v>
+      </c>
+      <c r="E3" s="115" t="s">
+        <v>38</v>
+      </c>
+      <c r="F3">
+        <v>1.1503209000220522</v>
+      </c>
+      <c r="G3" s="115" t="s">
+        <v>43</v>
+      </c>
+      <c r="H3" t="b">
+        <v>0</v>
+      </c>
+      <c r="I3" s="89">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" s="115" t="s">
+        <v>57</v>
+      </c>
+      <c r="B4" s="115" t="s">
+        <v>17</v>
+      </c>
+      <c r="C4" s="115" t="s">
+        <v>23</v>
+      </c>
+      <c r="D4" s="115" t="s">
         <v>19</v>
       </c>
-      <c r="C2" s="113" t="s">
-        <v>25</v>
-      </c>
-      <c r="D2" s="113" t="s">
-        <v>15</v>
-      </c>
-      <c r="E2" s="113" t="s">
-        <v>26</v>
-      </c>
-      <c r="F2">
-        <v>0.56264150002971292</v>
-      </c>
-      <c r="G2" s="113" t="s">
+      <c r="E4" s="115" t="s">
+        <v>32</v>
+      </c>
+      <c r="F4">
+        <v>0.38516549998894334</v>
+      </c>
+      <c r="G4" s="115" t="s">
+        <v>43</v>
+      </c>
+      <c r="H4" t="b">
+        <v>0</v>
+      </c>
+      <c r="I4" s="95">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" s="115" t="s">
+        <v>58</v>
+      </c>
+      <c r="B5" s="115" t="s">
+        <v>18</v>
+      </c>
+      <c r="C5" s="115" t="s">
+        <v>24</v>
+      </c>
+      <c r="D5" s="115" t="s">
+        <v>35</v>
+      </c>
+      <c r="E5" s="115" t="s">
+        <v>24</v>
+      </c>
+      <c r="F5">
+        <v>0.24058650003280491</v>
+      </c>
+      <c r="G5" s="115" t="s">
         <v>44</v>
-      </c>
-      <c r="H2" t="b">
-        <v>0</v>
-      </c>
-      <c r="I2" s="113" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="3">
-      <c r="A3" s="107" t="s">
-        <v>2</v>
-      </c>
-      <c r="B3" s="107" t="s">
-        <v>17</v>
-      </c>
-      <c r="C3" s="107" t="s">
-        <v>40</v>
-      </c>
-      <c r="D3" s="107" t="s">
-        <v>19</v>
-      </c>
-      <c r="E3" s="107" t="s">
-        <v>33</v>
-      </c>
-      <c r="F3">
-        <v>0.34822820010595024</v>
-      </c>
-      <c r="G3" s="107" t="s">
-        <v>43</v>
-      </c>
-      <c r="H3" t="b">
-        <v>0</v>
-      </c>
-      <c r="I3" s="89">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="4">
-      <c r="A4" s="107" t="s">
-        <v>3</v>
-      </c>
-      <c r="B4" s="107" t="s">
-        <v>19</v>
-      </c>
-      <c r="C4" s="107" t="s">
-        <v>32</v>
-      </c>
-      <c r="D4" s="107" t="s">
-        <v>15</v>
-      </c>
-      <c r="E4" s="107" t="s">
-        <v>23</v>
-      </c>
-      <c r="F4">
-        <v>0.22370430000592023</v>
-      </c>
-      <c r="G4" s="107" t="s">
-        <v>43</v>
-      </c>
-      <c r="H4" t="b">
-        <v>0</v>
-      </c>
-      <c r="I4" s="95">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="5">
-      <c r="A5" s="107" t="s">
-        <v>4</v>
-      </c>
-      <c r="B5" s="107" t="s">
-        <v>19</v>
-      </c>
-      <c r="C5" s="107" t="s">
-        <v>49</v>
-      </c>
-      <c r="D5" s="107" t="s">
-        <v>19</v>
-      </c>
-      <c r="E5" s="107" t="s">
-        <v>49</v>
-      </c>
-      <c r="F5">
-        <v>0.50990309996996075</v>
-      </c>
-      <c r="G5" s="107" t="s">
-        <v>43</v>
       </c>
       <c r="H5" t="b">
         <v>1</v>
       </c>
-      <c r="I5" s="107" t="s">
-        <v>48</v>
+      <c r="I5" s="107">
+        <v>0</v>
       </c>
     </row>
     <row r="6">

</xml_diff>